<commit_message>
Added the first 12 character cards.
</commit_message>
<xml_diff>
--- a/Character Card Names.xlsx
+++ b/Character Card Names.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19024"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UOSMSc\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jamie\CardGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B0FC8A96-50BC-4338-90CB-8B8BDEAE567E}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795" xr2:uid="{A7673FC6-4BB1-4C8A-8205-1D33638BF713}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12792" xr2:uid="{A7673FC6-4BB1-4C8A-8205-1D33638BF713}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -47,10 +46,6 @@
 (YouTuber)</t>
   </si>
   <si>
-    <t> H3H3
-(YouTuber)</t>
-  </si>
-  <si>
     <t>PewDiePie 
 (YouTuber)</t>
   </si>
@@ -434,13 +429,17 @@
   <si>
     <t> Michael Jackson
 (Singer)</t>
+  </si>
+  <si>
+    <t>Piers Morgan
+(Journalist)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -462,13 +461,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -480,10 +491,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -492,8 +504,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -808,476 +824,476 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{672643B3-0259-4B34-A44A-7AAAC951217D}">
   <dimension ref="A1:B69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0" xr3:uid="{65E0526C-65E5-51D3-A0DA-1784B8D51F9C}">
-      <selection activeCell="A54" sqref="A54"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="68.5703125" customWidth="1"/>
-    <col min="2" max="2" width="60.85546875" customWidth="1"/>
+    <col min="1" max="1" width="68.5546875" customWidth="1"/>
+    <col min="2" max="2" width="60.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="65.25" customHeight="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="65.25" customHeight="1">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="65.25" customHeight="1">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="65.25" customHeight="1">
-      <c r="A4" s="2" t="s">
+      <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2" t="s">
+    </row>
+    <row r="5" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="65.25" customHeight="1">
-      <c r="A5" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2" t="s">
+    </row>
+    <row r="6" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="65.25" customHeight="1">
-      <c r="A6" s="2" t="s">
+      <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="2" t="s">
+    </row>
+    <row r="7" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="65.25" customHeight="1">
-      <c r="A7" s="2" t="s">
+      <c r="B7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="3" t="s">
+    </row>
+    <row r="8" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="65.25" customHeight="1">
-      <c r="A8" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="2" t="s">
+    </row>
+    <row r="9" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="65.25" customHeight="1">
-      <c r="A9" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="2" t="s">
+    </row>
+    <row r="10" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="65.25" customHeight="1">
-      <c r="A10" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="2" t="s">
+    </row>
+    <row r="11" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" ht="65.25" customHeight="1">
-      <c r="A11" s="2" t="s">
+      <c r="B11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="2" t="s">
+    </row>
+    <row r="12" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" ht="65.25" customHeight="1">
-      <c r="A12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="2" t="s">
+    </row>
+    <row r="13" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" ht="65.25" customHeight="1">
-      <c r="A13" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="2" t="s">
+    </row>
+    <row r="14" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" ht="65.25" customHeight="1">
-      <c r="A14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="2" t="s">
+    </row>
+    <row r="15" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" ht="65.25" customHeight="1">
-      <c r="A15" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="2" t="s">
+    </row>
+    <row r="16" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" ht="65.25" customHeight="1">
-      <c r="A16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="2" t="s">
+    </row>
+    <row r="17" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="65.25" customHeight="1">
-      <c r="A17" s="2" t="s">
+      <c r="B17" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="2" t="s">
+    </row>
+    <row r="18" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="65.25" customHeight="1">
-      <c r="A18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="2" t="s">
+    </row>
+    <row r="19" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="65.25" customHeight="1">
-      <c r="A19" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="2" t="s">
+    </row>
+    <row r="20" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="65.25" customHeight="1">
-      <c r="A20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="2" t="s">
+    </row>
+    <row r="21" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="65.25" customHeight="1">
-      <c r="A21" s="2" t="s">
+      <c r="B21" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="2" t="s">
+    </row>
+    <row r="22" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" ht="65.25" customHeight="1">
-      <c r="A22" s="3" t="s">
+      <c r="B22" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="2" t="s">
+    </row>
+    <row r="23" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" ht="65.25" customHeight="1">
-      <c r="A23" s="2" t="s">
+      <c r="B23" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="2" t="s">
+    </row>
+    <row r="24" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" ht="65.25" customHeight="1">
-      <c r="A24" s="3" t="s">
+      <c r="B24" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="2" t="s">
+    </row>
+    <row r="25" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" ht="65.25" customHeight="1">
-      <c r="A25" s="2" t="s">
+      <c r="B25" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="2" t="s">
+    </row>
+    <row r="26" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" ht="65.25" customHeight="1">
-      <c r="A26" s="3" t="s">
+      <c r="B26" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="2" t="s">
+    </row>
+    <row r="27" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" ht="65.25" customHeight="1">
-      <c r="A27" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="2" t="s">
+    </row>
+    <row r="28" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" ht="65.25" customHeight="1">
-      <c r="A28" s="3" t="s">
+      <c r="B28" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B28" s="2" t="s">
+    </row>
+    <row r="29" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" ht="65.25" customHeight="1">
-      <c r="A29" s="2" t="s">
+      <c r="B29" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B29" s="2" t="s">
+    </row>
+    <row r="30" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" ht="65.25" customHeight="1">
-      <c r="A30" s="3" t="s">
+      <c r="B30" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B30" s="2" t="s">
+    </row>
+    <row r="31" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" ht="65.25" customHeight="1">
-      <c r="A31" s="2" t="s">
+      <c r="B31" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B31" s="2" t="s">
+    </row>
+    <row r="32" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" ht="65.25" customHeight="1">
-      <c r="A32" s="3" t="s">
+      <c r="B32" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B32" s="2" t="s">
+    </row>
+    <row r="33" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" ht="65.25" customHeight="1">
-      <c r="A33" s="2" t="s">
+      <c r="B33" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B33" s="2" t="s">
+    </row>
+    <row r="34" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" ht="65.25" customHeight="1">
-      <c r="A34" s="3" t="s">
+      <c r="B34" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B34" s="2" t="s">
+    </row>
+    <row r="35" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" ht="65.25" customHeight="1">
-      <c r="A35" s="2" t="s">
+      <c r="B35" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B35" s="2" t="s">
+    </row>
+    <row r="36" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" ht="65.25" customHeight="1">
-      <c r="A36" s="3" t="s">
+      <c r="B36" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B36" s="2" t="s">
+    </row>
+    <row r="37" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" ht="65.25" customHeight="1">
-      <c r="A37" s="2" t="s">
+      <c r="B37" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B37" s="2" t="s">
+    </row>
+    <row r="38" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" ht="65.25" customHeight="1">
-      <c r="A38" s="3" t="s">
+      <c r="B38" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B38" s="2" t="s">
+    </row>
+    <row r="39" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" ht="65.25" customHeight="1">
-      <c r="A39" s="2" t="s">
+      <c r="B39" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B39" s="2" t="s">
+    </row>
+    <row r="40" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="3" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" ht="65.25" customHeight="1">
-      <c r="A40" s="3" t="s">
+      <c r="B40" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B40" s="2" t="s">
+    </row>
+    <row r="41" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" ht="65.25" customHeight="1">
-      <c r="A41" s="2" t="s">
+      <c r="B41" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="2" t="s">
+    </row>
+    <row r="42" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="3" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" ht="65.25" customHeight="1">
-      <c r="A42" s="3" t="s">
+      <c r="B42" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B42" s="2" t="s">
+    </row>
+    <row r="43" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" ht="65.25" customHeight="1">
-      <c r="A43" s="2" t="s">
+      <c r="B43" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B43" s="2" t="s">
+    </row>
+    <row r="44" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="3" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" ht="65.25" customHeight="1">
-      <c r="A44" s="3" t="s">
+      <c r="B44" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B44" s="2" t="s">
+    </row>
+    <row r="45" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" ht="65.25" customHeight="1">
-      <c r="A45" s="2" t="s">
+      <c r="B45" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B45" s="2" t="s">
+    </row>
+    <row r="46" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="3" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" ht="65.25" customHeight="1">
-      <c r="A46" s="3" t="s">
+      <c r="B46" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B46" s="2" t="s">
+    </row>
+    <row r="47" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" ht="65.25" customHeight="1">
-      <c r="A47" s="2" t="s">
+      <c r="B47" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B47" s="2" t="s">
+    </row>
+    <row r="48" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="3" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" ht="65.25" customHeight="1">
-      <c r="A48" s="3" t="s">
+      <c r="B48" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B48" s="2" t="s">
+    </row>
+    <row r="49" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" ht="65.25" customHeight="1">
-      <c r="A49" s="2" t="s">
+      <c r="B49" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B49" s="2" t="s">
+    </row>
+    <row r="50" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="3" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" ht="65.25" customHeight="1">
-      <c r="A50" s="3" t="s">
+      <c r="B50" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B50" s="2" t="s">
+    </row>
+    <row r="51" spans="1:2" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="3" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" ht="60" customHeight="1">
-      <c r="A51" s="3" t="s">
+      <c r="B51" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B51" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="18.75">
+    </row>
+    <row r="52" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="B52" s="1"/>
     </row>
-    <row r="53" spans="1:2" ht="18.75">
+    <row r="53" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="B53" s="1"/>
     </row>
-    <row r="54" spans="1:2" ht="18.75">
+    <row r="54" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="B54" s="1"/>
     </row>
-    <row r="55" spans="1:2" ht="18.75">
+    <row r="55" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="B55" s="1"/>
     </row>
-    <row r="56" spans="1:2" ht="18.75">
+    <row r="56" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="B56" s="1"/>
     </row>
-    <row r="57" spans="1:2" ht="18.75">
+    <row r="57" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="B57" s="1"/>
     </row>
-    <row r="58" spans="1:2" ht="18.75">
+    <row r="58" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="B58" s="1"/>
     </row>
-    <row r="59" spans="1:2" ht="18.75">
+    <row r="59" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="B59" s="1"/>
     </row>
-    <row r="60" spans="1:2" ht="18.75">
+    <row r="60" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="B60" s="1"/>
     </row>
-    <row r="61" spans="1:2" ht="18.75">
+    <row r="61" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="B61" s="1"/>
     </row>
-    <row r="62" spans="1:2" ht="18.75">
+    <row r="62" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="B62" s="1"/>
     </row>
-    <row r="63" spans="1:2" ht="18.75">
+    <row r="63" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="B63" s="1"/>
     </row>
-    <row r="64" spans="1:2" ht="18.75">
+    <row r="64" spans="1:2" ht="18" x14ac:dyDescent="0.35">
       <c r="B64" s="1"/>
     </row>
-    <row r="65" spans="2:2" ht="18.75">
+    <row r="65" spans="2:2" ht="18" x14ac:dyDescent="0.35">
       <c r="B65" s="1"/>
     </row>
-    <row r="66" spans="2:2" ht="18.75">
+    <row r="66" spans="2:2" ht="18" x14ac:dyDescent="0.35">
       <c r="B66" s="1"/>
     </row>
-    <row r="67" spans="2:2" ht="18.75">
+    <row r="67" spans="2:2" ht="18" x14ac:dyDescent="0.35">
       <c r="B67" s="1"/>
     </row>
-    <row r="68" spans="2:2" ht="18.75">
+    <row r="68" spans="2:2" ht="18" x14ac:dyDescent="0.35">
       <c r="B68" s="1"/>
     </row>
-    <row r="69" spans="2:2" ht="18.75">
+    <row r="69" spans="2:2" ht="18" x14ac:dyDescent="0.35">
       <c r="B69" s="1"/>
     </row>
   </sheetData>
@@ -1287,12 +1303,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1461,19 +1474,46 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8DDFE37-0F73-4A35-9C2C-F1D43110B55D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2F909D3-661D-4764-A8D7-D6BBE358F248}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE5C778E-4439-499E-B95C-868199B12C9C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE5C778E-4439-499E-B95C-868199B12C9C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="e3e29f4b-52f7-45b4-9259-8578507ba859"/>
+    <ds:schemaRef ds:uri="43a8825b-007d-4564-b732-529cb2a5ef2d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2F909D3-661D-4764-A8D7-D6BBE358F248}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8DDFE37-0F73-4A35-9C2C-F1D43110B55D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
- Found a different font that's free to use commercially - Created 98 character cards & 20 situation cards for a total of 118 - Stumbled across a better program with which to make the card images, switched to it - Created a PDF of the cards
</commit_message>
<xml_diff>
--- a/Character Card Names.xlsx
+++ b/Character Card Names.xlsx
@@ -439,17 +439,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -493,20 +486,12 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -824,8 +809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{672643B3-0259-4B34-A44A-7AAAC951217D}">
   <dimension ref="A1:B69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -835,410 +820,410 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+      <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="A8" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="A9" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+      <c r="A10" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
+      <c r="A11" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
+      <c r="A12" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+      <c r="A13" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
+      <c r="A14" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+      <c r="A15" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
+      <c r="A16" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+      <c r="A17" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
+      <c r="A18" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+      <c r="A19" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
+      <c r="A20" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
+      <c r="A21" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
+      <c r="A22" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
+      <c r="A23" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
+      <c r="A24" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
+      <c r="A25" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
+      <c r="A26" t="s">
         <v>49</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
+      <c r="A27" t="s">
         <v>51</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
+      <c r="A28" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
+      <c r="A29" t="s">
         <v>55</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
+      <c r="A30" t="s">
         <v>57</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
+      <c r="A31" t="s">
         <v>59</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="3" t="s">
+      <c r="A32" t="s">
         <v>61</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
+      <c r="A33" t="s">
         <v>63</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="3" t="s">
+      <c r="A34" t="s">
         <v>65</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
+      <c r="A35" t="s">
         <v>67</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="3" t="s">
+      <c r="A36" t="s">
         <v>69</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="2" t="s">
+      <c r="A37" t="s">
         <v>71</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="3" t="s">
+      <c r="A38" t="s">
         <v>73</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="2" t="s">
+      <c r="A39" t="s">
         <v>75</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="3" t="s">
+      <c r="A40" t="s">
         <v>77</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="2" t="s">
+      <c r="A41" t="s">
         <v>79</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="3" t="s">
+      <c r="A42" t="s">
         <v>81</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="2" t="s">
+      <c r="A43" t="s">
         <v>83</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="3" t="s">
+      <c r="A44" t="s">
         <v>85</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="2" t="s">
+      <c r="A45" t="s">
         <v>87</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B45" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="3" t="s">
+      <c r="A46" t="s">
         <v>89</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="2" t="s">
+      <c r="A47" t="s">
         <v>91</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="3" t="s">
+      <c r="A48" t="s">
         <v>93</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B48" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="2" t="s">
+      <c r="A49" t="s">
         <v>95</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B49" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="3" t="s">
+      <c r="A50" t="s">
         <v>97</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B50" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="3" t="s">
+      <c r="A51" t="s">
         <v>99</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B51" t="s">
         <v>100</v>
       </c>
     </row>
@@ -1303,9 +1288,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1474,19 +1462,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2F909D3-661D-4764-A8D7-D6BBE358F248}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8DDFE37-0F73-4A35-9C2C-F1D43110B55D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1511,9 +1495,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8DDFE37-0F73-4A35-9C2C-F1D43110B55D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2F909D3-661D-4764-A8D7-D6BBE358F248}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>